<commit_message>
Week 10 and app updates
</commit_message>
<xml_diff>
--- a/NFL 2024 results.xlsx
+++ b/NFL 2024 results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mukappa/Documents/Coding/GitHub repos/not-for-long-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E7EBD5DF-A7E2-6C43-B7C0-C7CFCD5E639D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D35EBA-8023-F344-9FBB-2EF017D20BFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="7" xr2:uid="{A681E549-7284-2344-BB96-A3DD3BDA24DB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="9" xr2:uid="{A681E549-7284-2344-BB96-A3DD3BDA24DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,8 @@
     <sheet name="Week 6" sheetId="6" r:id="rId6"/>
     <sheet name="Week 7" sheetId="7" r:id="rId7"/>
     <sheet name="Week 8" sheetId="8" r:id="rId8"/>
+    <sheet name="Week 9" sheetId="9" r:id="rId9"/>
+    <sheet name="Week 10" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -43,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="43">
   <si>
     <t>Chiefs</t>
   </si>
@@ -169,6 +171,9 @@
   </si>
   <si>
     <t>Overtime</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> T</t>
   </si>
 </sst>
 </file>
@@ -960,6 +965,256 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{561AC108-CBE1-4542-8EBA-98FF1CFE7B95}">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2">
+        <v>35</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>16</v>
+      </c>
+      <c r="E7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14">
+        <v>27</v>
+      </c>
+      <c r="E14" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F81DF10-D5C0-E445-8F60-6B25F7CBDCED}">
   <dimension ref="A1:G17"/>
@@ -2183,7 +2438,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G1:G15"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2507,7 +2762,7 @@
         <v>16</v>
       </c>
       <c r="G14" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -3285,8 +3540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2552A93F-EF4C-B24B-807F-DF40A9CB6A76}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3685,4 +3940,387 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3995786B-9784-5E44-82DD-95CA8E85507B}">
+  <dimension ref="A1:G16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8">
+        <v>41</v>
+      </c>
+      <c r="E8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9">
+        <v>30</v>
+      </c>
+      <c r="E9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>27</v>
+      </c>
+      <c r="E10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>28</v>
+      </c>
+      <c r="E11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12">
+        <v>29</v>
+      </c>
+      <c r="E12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13">
+        <v>20</v>
+      </c>
+      <c r="E13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14">
+        <v>21</v>
+      </c>
+      <c r="E14" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>30</v>
+      </c>
+      <c r="E15" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" t="s">
+        <v>0</v>
+      </c>
+      <c r="G15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <v>10</v>
+      </c>
+      <c r="C16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16">
+        <v>41</v>
+      </c>
+      <c r="E16" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>